<commit_message>
update parts and tool list
</commit_message>
<xml_diff>
--- a/working parts and tool list.xlsx
+++ b/working parts and tool list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thela\Documents\Personal Projects\Clock\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A1C70B7-830D-4C47-93BB-7BB1D77EF97C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B25493C-C442-46D5-88C2-9589AFDFF4EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{332C783E-68BF-428D-95A1-31188BC60657}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="42">
   <si>
     <t>Part</t>
   </si>
@@ -145,6 +145,18 @@
   </si>
   <si>
     <t>Saw</t>
+  </si>
+  <si>
+    <t>Atmel ICE programmer</t>
+  </si>
+  <si>
+    <t>Hinges</t>
+  </si>
+  <si>
+    <t>Latch</t>
+  </si>
+  <si>
+    <t>Rubber feet</t>
   </si>
 </sst>
 </file>
@@ -537,16 +549,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A117CDF-FD20-4F3F-99B3-4056A7A71159}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="8.88671875" style="1"/>
@@ -793,91 +805,132 @@
         <v>22</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
+      <c r="A27" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>29</v>
+        <v>41</v>
+      </c>
+      <c r="B28" s="1">
+        <v>4</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A30" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>22</v>
       </c>
     </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="A33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>22</v>
-      </c>
+      <c r="A36" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C40" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="1" t="s">
         <v>22</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
+    <mergeCell ref="A36:C36"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A17:C17"/>
     <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A30:C30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>